<commit_message>
nsl kdd - HOPE ITS THE LAST TIME
</commit_message>
<xml_diff>
--- a/metrics-NSL-KDD.xlsx
+++ b/metrics-NSL-KDD.xlsx
@@ -604,16 +604,16 @@
         </is>
       </c>
       <c r="J2" t="n">
-        <v>0.9501397329547975</v>
+        <v>0.9500510136184181</v>
       </c>
       <c r="K2" t="n">
-        <v>0.9604921157511697</v>
+        <v>0.96</v>
       </c>
       <c r="L2" t="n">
-        <v>0.8608479577574157</v>
+        <v>0.86100326137599</v>
       </c>
       <c r="M2" t="n">
-        <v>0.9079443079443079</v>
+        <v>0.9078107090224332</v>
       </c>
     </row>
     <row r="3">
@@ -623,16 +623,16 @@
         </is>
       </c>
       <c r="J3" t="n">
-        <v>0.9347469280929779</v>
+        <v>0.9406467639622056</v>
       </c>
       <c r="K3" t="n">
-        <v>0.9577957980095835</v>
+        <v>0.9586405322783672</v>
       </c>
       <c r="L3" t="n">
-        <v>0.8071129057307035</v>
+        <v>0.8279235906196615</v>
       </c>
       <c r="M3" t="n">
-        <v>0.8760219131900546</v>
+        <v>0.8885</v>
       </c>
     </row>
     <row r="4">
@@ -642,16 +642,16 @@
         </is>
       </c>
       <c r="J4" t="n">
-        <v>0.9400257286075501</v>
+        <v>0.9417557556669476</v>
       </c>
       <c r="K4" t="n">
-        <v>0.9590326655838296</v>
+        <v>0.9591544249372984</v>
       </c>
       <c r="L4" t="n">
-        <v>0.8252834291038981</v>
+        <v>0.8314955738468707</v>
       </c>
       <c r="M4" t="n">
-        <v>0.8871452420701168</v>
+        <v>0.890774477996839</v>
       </c>
     </row>
     <row r="5">
@@ -661,16 +661,16 @@
         </is>
       </c>
       <c r="J5" t="n">
-        <v>0.9433970633899659</v>
+        <v>0.9435301423945349</v>
       </c>
       <c r="K5" t="n">
-        <v>0.9487224057013732</v>
+        <v>0.948905109489051</v>
       </c>
       <c r="L5" t="n">
-        <v>0.8476471501785992</v>
+        <v>0.8479577574157477</v>
       </c>
       <c r="M5" t="n">
-        <v>0.8953412073490813</v>
+        <v>0.8955958336750595</v>
       </c>
     </row>
     <row r="6">
@@ -680,16 +680,16 @@
         </is>
       </c>
       <c r="J6" t="n">
-        <v>0.8104511378254891</v>
+        <v>0.81031805882092</v>
       </c>
       <c r="K6" t="n">
-        <v>0.6181798341335661</v>
+        <v>0.6179775280898876</v>
       </c>
       <c r="L6" t="n">
         <v>0.8797949992234819</v>
       </c>
       <c r="M6" t="n">
-        <v>0.7261424085111837</v>
+        <v>0.7260028194284249</v>
       </c>
     </row>
   </sheetData>
@@ -740,16 +740,16 @@
         </is>
       </c>
       <c r="J2" t="n">
-        <v>0.9416670363305683</v>
+        <v>0.9440624584128111</v>
       </c>
       <c r="K2" t="n">
-        <v>0.9297215699429722</v>
+        <v>0.9383677615983745</v>
       </c>
       <c r="L2" t="n">
-        <v>0.8608479577574157</v>
+        <v>0.8606926541388414</v>
       </c>
       <c r="M2" t="n">
-        <v>0.8939601645028626</v>
+        <v>0.8978533819360064</v>
       </c>
     </row>
     <row r="3">
@@ -759,16 +759,16 @@
         </is>
       </c>
       <c r="J3" t="n">
-        <v>0.9472563545224681</v>
+        <v>0.9424655103579825</v>
       </c>
       <c r="K3" t="n">
-        <v>0.9637809187279152</v>
+        <v>0.958943234559086</v>
       </c>
       <c r="L3" t="n">
-        <v>0.8471812393228763</v>
+        <v>0.8342910389812083</v>
       </c>
       <c r="M3" t="n">
-        <v>0.9017274154888834</v>
+        <v>0.8922846939622954</v>
       </c>
     </row>
     <row r="4">
@@ -778,16 +778,16 @@
         </is>
       </c>
       <c r="J4" t="n">
-        <v>0.9479217495453134</v>
+        <v>0.9430421860444483</v>
       </c>
       <c r="K4" t="n">
-        <v>0.9622475856014048</v>
+        <v>0.9592018528416176</v>
       </c>
       <c r="L4" t="n">
-        <v>0.851063829787234</v>
+        <v>0.8361546824041001</v>
       </c>
       <c r="M4" t="n">
-        <v>0.903247074336575</v>
+        <v>0.8934616661135081</v>
       </c>
     </row>
     <row r="5">
@@ -797,16 +797,16 @@
         </is>
       </c>
       <c r="J5" t="n">
-        <v>0.9096837155658075</v>
+        <v>0.9114137426252051</v>
       </c>
       <c r="K5" t="n">
-        <v>0.8912386706948641</v>
+        <v>0.9000360230547551</v>
       </c>
       <c r="L5" t="n">
-        <v>0.7788476471501786</v>
+        <v>0.7760521820158409</v>
       </c>
       <c r="M5" t="n">
-        <v>0.8312613956572187</v>
+        <v>0.8334584271536986</v>
       </c>
     </row>
     <row r="6">
@@ -816,16 +816,16 @@
         </is>
       </c>
       <c r="J6" t="n">
-        <v>0.8814709665971698</v>
+        <v>0.8760590870780287</v>
       </c>
       <c r="K6" t="n">
-        <v>0.8161826422695988</v>
+        <v>0.8130905342724618</v>
       </c>
       <c r="L6" t="n">
-        <v>0.7550861935083087</v>
+        <v>0.7350520267122224</v>
       </c>
       <c r="M6" t="n">
-        <v>0.7844465956760244</v>
+        <v>0.7721044045676998</v>
       </c>
     </row>
   </sheetData>
@@ -876,16 +876,16 @@
         </is>
       </c>
       <c r="J2" t="n">
-        <v>0.9500510136184181</v>
+        <v>0.9503171716275562</v>
       </c>
       <c r="K2" t="n">
-        <v>0.96</v>
+        <v>0.9608386761393173</v>
       </c>
       <c r="L2" t="n">
-        <v>0.86100326137599</v>
+        <v>0.8611585649945643</v>
       </c>
       <c r="M2" t="n">
-        <v>0.9078107090224332</v>
+        <v>0.9082719082719082</v>
       </c>
     </row>
     <row r="3">
@@ -895,16 +895,16 @@
         </is>
       </c>
       <c r="J3" t="n">
-        <v>0.9404693252894468</v>
+        <v>0.9406024042940159</v>
       </c>
       <c r="K3" t="n">
-        <v>0.9586107612020874</v>
+        <v>0.9584681769147788</v>
       </c>
       <c r="L3" t="n">
-        <v>0.8273023761453642</v>
+        <v>0.8279235906196615</v>
       </c>
       <c r="M3" t="n">
-        <v>0.8881293764588196</v>
+        <v>0.8884259645029581</v>
       </c>
     </row>
     <row r="4">
@@ -914,16 +914,16 @@
         </is>
       </c>
       <c r="J4" t="n">
-        <v>0.9392272545801358</v>
+        <v>0.9405580446258262</v>
       </c>
       <c r="K4" t="n">
-        <v>0.9584011575330078</v>
+        <v>0.9587907144142523</v>
       </c>
       <c r="L4" t="n">
-        <v>0.8229538748252835</v>
+        <v>0.8274576797639385</v>
       </c>
       <c r="M4" t="n">
-        <v>0.8855280748663102</v>
+        <v>0.8882960986995665</v>
       </c>
     </row>
     <row r="5">
@@ -933,16 +933,16 @@
         </is>
       </c>
       <c r="J5" t="n">
-        <v>0.9453488887903119</v>
+        <v>0.9454819677948809</v>
       </c>
       <c r="K5" t="n">
-        <v>0.9582819926069354</v>
+        <v>0.9579817158931083</v>
       </c>
       <c r="L5" t="n">
-        <v>0.8454728995185588</v>
+        <v>0.8462494176114304</v>
       </c>
       <c r="M5" t="n">
-        <v>0.8983498349834984</v>
+        <v>0.8986558918116599</v>
       </c>
     </row>
     <row r="6">
@@ -952,16 +952,16 @@
         </is>
       </c>
       <c r="J6" t="n">
-        <v>0.904050037705718</v>
+        <v>0.9023200106463204</v>
       </c>
       <c r="K6" t="n">
-        <v>0.8781393703572692</v>
+        <v>0.8710807496934665</v>
       </c>
       <c r="L6" t="n">
-        <v>0.7710824662214629</v>
+        <v>0.7723248951700574</v>
       </c>
       <c r="M6" t="n">
-        <v>0.8211361944926817</v>
+        <v>0.8187355943365163</v>
       </c>
     </row>
   </sheetData>
@@ -1284,16 +1284,16 @@
         </is>
       </c>
       <c r="J2" t="n">
-        <v>0.9476112318679857</v>
+        <v>0.9471676351860888</v>
       </c>
       <c r="K2" t="n">
-        <v>0.9570584144645341</v>
+        <v>0.9555555555555556</v>
       </c>
       <c r="L2" t="n">
-        <v>0.8549464202515918</v>
+        <v>0.8547911166330175</v>
       </c>
       <c r="M2" t="n">
-        <v>0.9031252563366418</v>
+        <v>0.9023690466431674</v>
       </c>
     </row>
     <row r="3">
@@ -1303,16 +1303,16 @@
         </is>
       </c>
       <c r="J3" t="n">
-        <v>0.9290688905646985</v>
+        <v>0.9330169010335803</v>
       </c>
       <c r="K3" t="n">
-        <v>0.959203036053131</v>
+        <v>0.9597090095131505</v>
       </c>
       <c r="L3" t="n">
-        <v>0.7850597918931511</v>
+        <v>0.7990371175648393</v>
       </c>
       <c r="M3" t="n">
-        <v>0.8634383807327696</v>
+        <v>0.8720338983050847</v>
       </c>
     </row>
     <row r="4">
@@ -1322,16 +1322,16 @@
         </is>
       </c>
       <c r="J4" t="n">
-        <v>0.9331056203699596</v>
+        <v>0.9342589717428914</v>
       </c>
       <c r="K4" t="n">
-        <v>0.9598955418765156</v>
+        <v>0.9599183521989237</v>
       </c>
       <c r="L4" t="n">
-        <v>0.7991924211834136</v>
+        <v>0.80338561888492</v>
       </c>
       <c r="M4" t="n">
-        <v>0.8722033898305085</v>
+        <v>0.87470409198512</v>
       </c>
     </row>
     <row r="5">
@@ -1341,16 +1341,16 @@
         </is>
       </c>
       <c r="J5" t="n">
-        <v>0.9386062192254802</v>
+        <v>0.939759570598412</v>
       </c>
       <c r="K5" t="n">
-        <v>0.9379656905215734</v>
+        <v>0.939152981849611</v>
       </c>
       <c r="L5" t="n">
-        <v>0.8406584873427551</v>
+        <v>0.8437645597142414</v>
       </c>
       <c r="M5" t="n">
-        <v>0.8866502866502867</v>
+        <v>0.8889070680628273</v>
       </c>
     </row>
     <row r="6">
@@ -1360,16 +1360,16 @@
         </is>
       </c>
       <c r="J6" t="n">
-        <v>0.8860400124207071</v>
+        <v>0.8780109124783747</v>
       </c>
       <c r="K6" t="n">
-        <v>0.8140214216163584</v>
+        <v>0.7769103738177451</v>
       </c>
       <c r="L6" t="n">
-        <v>0.7790029507687529</v>
+        <v>0.8036962261220686</v>
       </c>
       <c r="M6" t="n">
-        <v>0.7961272914848028</v>
+        <v>0.7900763358778624</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
nsl kdd - HOPE ITS THE LAST TIMEE
</commit_message>
<xml_diff>
--- a/metrics-NSL-KDD.xlsx
+++ b/metrics-NSL-KDD.xlsx
@@ -431,7 +431,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="I1:M6"/>
+  <dimension ref="I1:N6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -460,6 +460,11 @@
           <t>F1 Score</t>
         </is>
       </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>False alarm rate</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="I2" s="1" t="inlineStr">
@@ -479,6 +484,9 @@
       <c r="M2" t="n">
         <v>0.9075726565697912</v>
       </c>
+      <c r="N2" t="n">
+        <v>0.01446845504222553</v>
+      </c>
     </row>
     <row r="3">
       <c r="I3" s="1" t="inlineStr">
@@ -498,6 +506,9 @@
       <c r="M3" t="n">
         <v>0.8940298507462686</v>
       </c>
+      <c r="N3" t="n">
+        <v>0.01428216592151018</v>
+      </c>
     </row>
     <row r="4">
       <c r="I4" s="1" t="inlineStr">
@@ -517,6 +528,9 @@
       <c r="M4" t="n">
         <v>0.8919727438923052</v>
       </c>
+      <c r="N4" t="n">
+        <v>0.01415797317436662</v>
+      </c>
     </row>
     <row r="5">
       <c r="I5" s="1" t="inlineStr">
@@ -536,6 +550,9 @@
       <c r="M5" t="n">
         <v>0.8743743333059818</v>
       </c>
+      <c r="N5" t="n">
+        <v>0.02608047690014903</v>
+      </c>
     </row>
     <row r="6">
       <c r="I6" s="1" t="inlineStr">
@@ -554,6 +571,9 @@
       </c>
       <c r="M6" t="n">
         <v>0.5237028250076886</v>
+      </c>
+      <c r="N6" t="n">
+        <v>0.6434426229508197</v>
       </c>
     </row>
   </sheetData>
@@ -567,7 +587,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="I1:M6"/>
+  <dimension ref="I1:N6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -596,6 +616,11 @@
           <t>F1 Score</t>
         </is>
       </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> false_alarm_rate</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="I2" s="1" t="inlineStr">
@@ -615,6 +640,9 @@
       <c r="M2" t="n">
         <v>0.9078107090224332</v>
       </c>
+      <c r="N2" t="n">
+        <v>0.01434426229508197</v>
+      </c>
     </row>
     <row r="3">
       <c r="I3" s="1" t="inlineStr">
@@ -634,6 +662,9 @@
       <c r="M3" t="n">
         <v>0.8885</v>
       </c>
+      <c r="N3" t="n">
+        <v>0.01428216592151018</v>
+      </c>
     </row>
     <row r="4">
       <c r="I4" s="1" t="inlineStr">
@@ -653,6 +684,9 @@
       <c r="M4" t="n">
         <v>0.890774477996839</v>
       </c>
+      <c r="N4" t="n">
+        <v>0.01415797317436662</v>
+      </c>
     </row>
     <row r="5">
       <c r="I5" s="1" t="inlineStr">
@@ -672,6 +706,9 @@
       <c r="M5" t="n">
         <v>0.8955958336750595</v>
       </c>
+      <c r="N5" t="n">
+        <v>0.01825633383010432</v>
+      </c>
     </row>
     <row r="6">
       <c r="I6" s="1" t="inlineStr">
@@ -690,6 +727,9 @@
       </c>
       <c r="M6" t="n">
         <v>0.7260028194284249</v>
+      </c>
+      <c r="N6" t="n">
+        <v>0.2174615002483855</v>
       </c>
     </row>
   </sheetData>
@@ -703,7 +743,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="I1:M6"/>
+  <dimension ref="I1:N6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -732,6 +772,11 @@
           <t>F1 Score</t>
         </is>
       </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>false_alarm_rate</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="I2" s="1" t="inlineStr">
@@ -751,6 +796,9 @@
       <c r="M2" t="n">
         <v>0.8978533819360064</v>
       </c>
+      <c r="N2" t="n">
+        <v>0.02260307998012916</v>
+      </c>
     </row>
     <row r="3">
       <c r="I3" s="1" t="inlineStr">
@@ -770,6 +818,9 @@
       <c r="M3" t="n">
         <v>0.8922846939622954</v>
       </c>
+      <c r="N3" t="n">
+        <v>0.01428216592151018</v>
+      </c>
     </row>
     <row r="4">
       <c r="I4" s="1" t="inlineStr">
@@ -789,6 +840,9 @@
       <c r="M4" t="n">
         <v>0.8934616661135081</v>
       </c>
+      <c r="N4" t="n">
+        <v>0.0142200695479384</v>
+      </c>
     </row>
     <row r="5">
       <c r="I5" s="1" t="inlineStr">
@@ -808,6 +862,9 @@
       <c r="M5" t="n">
         <v>0.8334584271536986</v>
       </c>
+      <c r="N5" t="n">
+        <v>0.03446348733233979</v>
+      </c>
     </row>
     <row r="6">
       <c r="I6" s="1" t="inlineStr">
@@ -826,6 +883,9 @@
       </c>
       <c r="M6" t="n">
         <v>0.7721044045676998</v>
+      </c>
+      <c r="N6" t="n">
+        <v>0.06756085444610035</v>
       </c>
     </row>
   </sheetData>
@@ -839,7 +899,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="I1:M6"/>
+  <dimension ref="I1:N6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -868,6 +928,11 @@
           <t>F1 Score</t>
         </is>
       </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>false_alarm_rate</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="I2" s="1" t="inlineStr">
@@ -887,6 +952,9 @@
       <c r="M2" t="n">
         <v>0.9082719082719082</v>
       </c>
+      <c r="N2" t="n">
+        <v>0.01403378042722305</v>
+      </c>
     </row>
     <row r="3">
       <c r="I3" s="1" t="inlineStr">
@@ -906,6 +974,9 @@
       <c r="M3" t="n">
         <v>0.8884259645029581</v>
       </c>
+      <c r="N3" t="n">
+        <v>0.01434426229508197</v>
+      </c>
     </row>
     <row r="4">
       <c r="I4" s="1" t="inlineStr">
@@ -925,6 +996,9 @@
       <c r="M4" t="n">
         <v>0.8882960986995665</v>
       </c>
+      <c r="N4" t="n">
+        <v>0.0142200695479384</v>
+      </c>
     </row>
     <row r="5">
       <c r="I5" s="1" t="inlineStr">
@@ -944,6 +1018,9 @@
       <c r="M5" t="n">
         <v>0.8986558918116599</v>
       </c>
+      <c r="N5" t="n">
+        <v>0.01484103328365623</v>
+      </c>
     </row>
     <row r="6">
       <c r="I6" s="1" t="inlineStr">
@@ -962,6 +1039,9 @@
       </c>
       <c r="M6" t="n">
         <v>0.8187355943365163</v>
+      </c>
+      <c r="N6" t="n">
+        <v>0.04570293094883259</v>
       </c>
     </row>
   </sheetData>
@@ -975,7 +1055,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="I1:M6"/>
+  <dimension ref="I1:N6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1004,6 +1084,11 @@
           <t>F1 Score</t>
         </is>
       </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> false_alarm_rate</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="I2" s="1" t="inlineStr">
@@ -1023,6 +1108,9 @@
       <c r="M2" t="n">
         <v>0.9026736224323443</v>
       </c>
+      <c r="N2" t="n">
+        <v>0.01813214108296075</v>
+      </c>
     </row>
     <row r="3">
       <c r="I3" s="1" t="inlineStr">
@@ -1042,6 +1130,9 @@
       <c r="M3" t="n">
         <v>0.8919773635153129</v>
       </c>
+      <c r="N3" t="n">
+        <v>0.01353700943864878</v>
+      </c>
     </row>
     <row r="4">
       <c r="I4" s="1" t="inlineStr">
@@ -1061,6 +1152,9 @@
       <c r="M4" t="n">
         <v>0.8947936560657644</v>
       </c>
+      <c r="N4" t="n">
+        <v>0.01341281669150522</v>
+      </c>
     </row>
     <row r="5">
       <c r="I5" s="1" t="inlineStr">
@@ -1080,6 +1174,9 @@
       <c r="M5" t="n">
         <v>0.8257575757575758</v>
       </c>
+      <c r="N5" t="n">
+        <v>0.05253353204172876</v>
+      </c>
     </row>
     <row r="6">
       <c r="I6" s="1" t="inlineStr">
@@ -1098,6 +1195,9 @@
       </c>
       <c r="M6" t="n">
         <v>0.7665278303672851</v>
+      </c>
+      <c r="N6" t="n">
+        <v>0.1058743169398907</v>
       </c>
     </row>
   </sheetData>
@@ -1111,7 +1211,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="I1:M6"/>
+  <dimension ref="I1:N6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1140,6 +1240,11 @@
           <t>F1 Score</t>
         </is>
       </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> false_alarm_rate</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="I2" s="1" t="inlineStr">
@@ -1159,6 +1264,9 @@
       <c r="M2" t="n">
         <v>0.906533649521629</v>
       </c>
+      <c r="N2" t="n">
+        <v>0.0153378042722305</v>
+      </c>
     </row>
     <row r="3">
       <c r="I3" s="1" t="inlineStr">
@@ -1178,6 +1286,9 @@
       <c r="M3" t="n">
         <v>0.8640668999061354</v>
       </c>
+      <c r="N3" t="n">
+        <v>0.013474913065077</v>
+      </c>
     </row>
     <row r="4">
       <c r="I4" s="1" t="inlineStr">
@@ -1197,6 +1308,9 @@
       <c r="M4" t="n">
         <v>0.8754436369781984</v>
       </c>
+      <c r="N4" t="n">
+        <v>0.01335072031793343</v>
+      </c>
     </row>
     <row r="5">
       <c r="I5" s="1" t="inlineStr">
@@ -1216,6 +1330,9 @@
       <c r="M5" t="n">
         <v>0.7604506858262572</v>
       </c>
+      <c r="N5" t="n">
+        <v>0.07153502235469449</v>
+      </c>
     </row>
     <row r="6">
       <c r="I6" s="1" t="inlineStr">
@@ -1234,6 +1351,9 @@
       </c>
       <c r="M6" t="n">
         <v>0.8043980559317983</v>
+      </c>
+      <c r="N6" t="n">
+        <v>0.06607054148037754</v>
       </c>
     </row>
   </sheetData>
@@ -1247,7 +1367,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="I1:M6"/>
+  <dimension ref="I1:N6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1276,6 +1396,11 @@
           <t>F1 Score</t>
         </is>
       </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>false_alarm_rate</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="I2" s="1" t="inlineStr">
@@ -1295,6 +1420,9 @@
       <c r="M2" t="n">
         <v>0.9023690466431674</v>
       </c>
+      <c r="N2" t="n">
+        <v>0.01589667163437655</v>
+      </c>
     </row>
     <row r="3">
       <c r="I3" s="1" t="inlineStr">
@@ -1314,6 +1442,9 @@
       <c r="M3" t="n">
         <v>0.8720338983050847</v>
       </c>
+      <c r="N3" t="n">
+        <v>0.01341281669150522</v>
+      </c>
     </row>
     <row r="4">
       <c r="I4" s="1" t="inlineStr">
@@ -1333,6 +1464,9 @@
       <c r="M4" t="n">
         <v>0.87470409198512</v>
       </c>
+      <c r="N4" t="n">
+        <v>0.01341281669150522</v>
+      </c>
     </row>
     <row r="5">
       <c r="I5" s="1" t="inlineStr">
@@ -1352,6 +1486,9 @@
       <c r="M5" t="n">
         <v>0.8889070680628273</v>
       </c>
+      <c r="N5" t="n">
+        <v>0.02185792349726776</v>
+      </c>
     </row>
     <row r="6">
       <c r="I6" s="1" t="inlineStr">
@@ -1370,6 +1507,9 @@
       </c>
       <c r="M6" t="n">
         <v>0.7900763358778624</v>
+      </c>
+      <c r="N6" t="n">
+        <v>0.09227521112767015</v>
       </c>
     </row>
   </sheetData>

</xml_diff>